<commit_message>
Add region maps and tracks.
</commit_message>
<xml_diff>
--- a/data/plan.xlsx
+++ b/data/plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -175,7 +175,10 @@
     <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) -- Col de Fontaines (н/к, 2696) -- Mont-Perron -- camping Glair</t>
   </si>
   <si>
-    <t xml:space="preserve">+250,-1400</t>
+    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) – вер. Becca Trecare (н/к,  3032) – Col de Fontaines (н/к, 2696) -- Mont-Perron -- camping Glair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+450,-1600</t>
   </si>
   <si>
     <t xml:space="preserve">13b</t>
@@ -315,8 +318,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -725,7 +728,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -736,7 +739,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>17.4</v>
@@ -748,7 +751,7 @@
         <v>2773</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>7</v>
@@ -756,16 +759,16 @@
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>16.9</v>
@@ -785,10 +788,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,10 +799,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add pass description. Add maps and height graph
</commit_message>
<xml_diff>
--- a/data/plan.xlsx
+++ b/data/plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -46,7 +46,10 @@
     <t xml:space="preserve">Δh, м</t>
   </si>
   <si>
-    <t xml:space="preserve">T, ч</t>
+    <t xml:space="preserve">ГХВ, ч</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЧХВ, ч</t>
   </si>
   <si>
     <t xml:space="preserve">2019-07-13</t>
@@ -61,13 +64,25 @@
     <t xml:space="preserve">Подход под пер. Passo di Campo (2180 н/к). Озеро Lagho di Campo (2290)</t>
   </si>
   <si>
+    <t xml:space="preserve">07:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02:44</t>
+  </si>
+  <si>
     <t xml:space="preserve">2019-07-15</t>
   </si>
   <si>
     <t xml:space="preserve">пер. Passo di Pontimia (н/к, 2387) -- пос. Gmeinalp (1850) -- подход под пер. Zwischenbergenpass</t>
   </si>
   <si>
-    <t xml:space="preserve">+150, -550, + 550</t>
+    <t xml:space="preserve">'+580 / -680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03:04</t>
   </si>
   <si>
     <t xml:space="preserve">2019-07-16</t>
@@ -76,7 +91,13 @@
     <t xml:space="preserve">пер. Zwischenbergen (1Б, 3287) -- Almageller Hutte (2900) -- Almagelleralp (2200)</t>
   </si>
   <si>
-    <t xml:space="preserve">+1000, -1000</t>
+    <t xml:space="preserve">'+1100/ -1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:54</t>
   </si>
   <si>
     <t xml:space="preserve">2019-07-17</t>
@@ -85,6 +106,12 @@
     <t xml:space="preserve">Almagelleralp -- Saas-Almagel -- Mischabel camping / Kappelenweg</t>
   </si>
   <si>
+    <t xml:space="preserve">02:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01:54</t>
+  </si>
+  <si>
     <t xml:space="preserve">5a</t>
   </si>
   <si>
@@ -94,6 +121,12 @@
     <t xml:space="preserve">Am Kapellenweg -- Mischabelhutte</t>
   </si>
   <si>
+    <t xml:space="preserve">09:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:39</t>
+  </si>
+  <si>
     <t xml:space="preserve">6a</t>
   </si>
   <si>
@@ -103,7 +136,13 @@
     <t xml:space="preserve">Mischabelhutte -- Windjoch (1Б, 3850, сн-ск) -- вер. Ulrichshorn (1Б, 3925) -- пер. Riedpass (1Б, 3555) -- вер. P3644 (1А, сн) -- Bordierhutte</t>
   </si>
   <si>
-    <t xml:space="preserve">+600,-1100</t>
+    <t xml:space="preserve">+600,-900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04:40</t>
   </si>
   <si>
     <t xml:space="preserve">7a</t>
@@ -115,6 +154,15 @@
     <t xml:space="preserve">Bordierhutte -- пер. 2664 (н/к) -- Europahutte -- Tasch</t>
   </si>
   <si>
+    <t xml:space="preserve">'+500/-2120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:52</t>
+  </si>
+  <si>
     <t xml:space="preserve">2019-07-21</t>
   </si>
   <si>
@@ -127,6 +175,12 @@
     <t xml:space="preserve">Zermatt -- Furi -- Trockener weg (подъёмник) -- подход по Breithorn</t>
   </si>
   <si>
+    <t xml:space="preserve">08:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04:42</t>
+  </si>
+  <si>
     <t xml:space="preserve">10a</t>
   </si>
   <si>
@@ -136,7 +190,13 @@
     <t xml:space="preserve">вер. Breithorn (1Б, 4164, снежн.) -- Bivacco Rossi e Volante (3700) -- оз. 2740</t>
   </si>
   <si>
-    <t xml:space="preserve">+360, - 1300</t>
+    <t xml:space="preserve">+200, - 1200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02:58</t>
   </si>
   <si>
     <t xml:space="preserve">11a</t>
@@ -148,7 +208,13 @@
     <t xml:space="preserve">оз. 2740 -- оз. Lago Blu (2200) -- Rifugio Guide of Frahey (2100) --р. Torrente Curtod -- пер. Сolletto di Nano (1А, 2650)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1000,+900</t>
+    <t xml:space="preserve">-1000,+860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04:56</t>
   </si>
   <si>
     <t xml:space="preserve">12a</t>
@@ -178,13 +244,25 @@
     <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) – вер. Becca Trecare (н/к,  3032) – Col de Fontaines (н/к, 2696) -- Mont-Perron -- camping Glair</t>
   </si>
   <si>
-    <t xml:space="preserve">+450,-1600</t>
+    <t xml:space="preserve">+350,-1600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03:36</t>
   </si>
   <si>
     <t xml:space="preserve">13b</t>
   </si>
   <si>
     <t xml:space="preserve">camping Glair -- St. Vincent (Casino)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01:30</t>
   </si>
   <si>
     <t xml:space="preserve">2019-07-27</t>
@@ -203,15 +281,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -233,11 +313,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,7 +364,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +379,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -316,18 +402,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="32.79"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -355,19 +446,22 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1250</v>
@@ -376,224 +470,242 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>2290</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>2290</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2286</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>2286.37</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1080</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>10.1</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>2387</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2176</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2374.16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>2200</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>3287</v>
+        <v>22</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2275.54</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>3268.71</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>2200</v>
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1572</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>2197.9</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>-700</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-650</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>3300</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>3300</v>
+        <v>32</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3323</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>3325.05</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>1700</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1760</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>2900</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>3925</v>
+        <v>37</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>3034</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>3921.53</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>1608</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>2865</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>-1200</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1424</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>3037.44</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1608</v>
@@ -604,123 +716,122 @@
       <c r="H10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>1608</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>3800</v>
+        <v>50</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>3812</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>3812.43</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>2200</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2400</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>2740</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>4164</v>
+        <v>55</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2747</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>3824.75</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>2590</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>2740</v>
+        <v>61</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>2732.39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -728,47 +839,50 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>17.4</v>
+        <v>73</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>11</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>1350</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>2773</v>
+        <v>2586</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>2768.04</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>16.9</v>
@@ -779,8 +893,11 @@
       <c r="H17" s="2" t="n">
         <v>-900</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <v>6</v>
+      <c r="I17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,21 +905,21 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix distance. Extended and correct info part of report.
</commit_message>
<xml_diff>
--- a/data/plan.xlsx
+++ b/data/plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -55,13 +55,13 @@
     <t xml:space="preserve">2019-07-13</t>
   </si>
   <si>
-    <t xml:space="preserve">Прилет в Milan в 13:40. Переезд до Domodosolla. Аренда авто до Bognanco (Yolki Palki)</t>
+    <t xml:space="preserve">Заезд Milan – Domodosolla -- Bognanco – кэмпинг Yolki Palki</t>
   </si>
   <si>
     <t xml:space="preserve">2019-07-14</t>
   </si>
   <si>
-    <t xml:space="preserve">Подход под пер. Passo di Campo (2180 н/к). Озеро Lagho di Campo (2290)</t>
+    <t xml:space="preserve">пер. Passo di Campo (2180 н/к) – оз. Lagho di Campo (2290)</t>
   </si>
   <si>
     <t xml:space="preserve">07:03</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">2019-07-15</t>
   </si>
   <si>
-    <t xml:space="preserve">пер. Passo di Pontimia (н/к, 2387) -- пос. Gmeinalp (1850) -- подход под пер. Zwischenbergenpass</t>
+    <t xml:space="preserve">пер. Passo di Pontimia (н/к, 2387) -- пос. Gmeinalp (1850) – ур. Galki (2300)</t>
   </si>
   <si>
     <t xml:space="preserve">'+580 / -680</t>
@@ -103,7 +103,10 @@
     <t xml:space="preserve">2019-07-17</t>
   </si>
   <si>
-    <t xml:space="preserve">Almagelleralp -- Saas-Almagel -- Mischabel camping / Kappelenweg</t>
+    <t xml:space="preserve">Almagelleralp – дер. Saas-Almagel -- Mischabel camping / Kappelenweg – полуднёвка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almagelleralp – дер. Saas-Almagel – кемпирг “Am Kappelenweg” – полуднёвка</t>
   </si>
   <si>
     <t xml:space="preserve">02:36</t>
@@ -118,7 +121,7 @@
     <t xml:space="preserve">2019-07-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Am Kapellenweg -- Mischabelhutte</t>
+    <t xml:space="preserve">дер. Saas-Fee – хиж. Mischabelhutte</t>
   </si>
   <si>
     <t xml:space="preserve">09:55</t>
@@ -133,7 +136,7 @@
     <t xml:space="preserve">2019-07-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Mischabelhutte -- Windjoch (1Б, 3850, сн-ск) -- вер. Ulrichshorn (1Б, 3925) -- пер. Riedpass (1Б, 3555) -- вер. P3644 (1А, сн) -- Bordierhutte</t>
+    <t xml:space="preserve">Хиж. Mischabelhutte -- Windjoch (1Б, 3850, сн-л) -- вер. Ulrichshorn (1Б, 3925) – хиж. Bordierhutte</t>
   </si>
   <si>
     <t xml:space="preserve">+600,-900</t>
@@ -151,7 +154,10 @@
     <t xml:space="preserve">2019-07-20</t>
   </si>
   <si>
-    <t xml:space="preserve">Bordierhutte -- пер. 2664 (н/к) -- Europahutte -- Tasch</t>
+    <t xml:space="preserve">Хиж. Bordierhutte -- пер. 2664 (н/к) – хиж. Europahutte – кемпинг Tasch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хиж. Bordierhutte -- пер. 2664 (н/к) – хиж. Europahutte – кемпинг Rand</t>
   </si>
   <si>
     <t xml:space="preserve">'+500/-2120</t>
@@ -172,7 +178,10 @@
     <t xml:space="preserve">2019-07-22</t>
   </si>
   <si>
-    <t xml:space="preserve">Zermatt -- Furi -- Trockener weg (подъёмник) -- подход по Breithorn</t>
+    <t xml:space="preserve">Zermatt – ст. Furi – ст. Trockener Steg (переезд на подъёмнике) – подход по Breithorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zermatt – ст. Furi – ст. Trockener Steg (переезд на подъёмнике *) – пер. P3824</t>
   </si>
   <si>
     <t xml:space="preserve">08:41</t>
@@ -187,7 +196,7 @@
     <t xml:space="preserve">2019-07-23</t>
   </si>
   <si>
-    <t xml:space="preserve">вер. Breithorn (1Б, 4164, снежн.) -- Bivacco Rossi e Volante (3700) -- оз. 2740</t>
+    <t xml:space="preserve">вер. Breithorn (1Б, 4164, снежн.) -- развилка Bivacco Rossi e Volante (3700) -- оз. 2740</t>
   </si>
   <si>
     <t xml:space="preserve">+200, - 1200</t>
@@ -205,7 +214,7 @@
     <t xml:space="preserve">2019-07-24</t>
   </si>
   <si>
-    <t xml:space="preserve">оз. 2740 -- оз. Lago Blu (2200) -- Rifugio Guide of Frahey (2100) --р. Torrente Curtod -- пер. Сolletto di Nano (1А, 2650)</t>
+    <t xml:space="preserve">оз. 2740 – дол. Verraz  – дер. Blanchard -- пер. Сolletto di Nano (1А, 2650)</t>
   </si>
   <si>
     <t xml:space="preserve">-1000,+860</t>
@@ -223,7 +232,7 @@
     <t xml:space="preserve">2019-07-25</t>
   </si>
   <si>
-    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) -- р. Torrente Chamois (1400) -- дер. Chamois -- дер. Nuarsazz -- Camping Cervino (1130)</t>
+    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) – дер. Chamois -- дер. Nuarsaz – кемп. Cervino (1130)</t>
   </si>
   <si>
     <t xml:space="preserve">13a</t>
@@ -238,10 +247,10 @@
     <t xml:space="preserve">12b</t>
   </si>
   <si>
-    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) -- Col de Fontaines (н/к, 2696) -- Mont-Perron -- camping Glair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) – вер. Becca Trecare (н/к,  3032) – Col de Fontaines (н/к, 2696) -- Mont-Perron -- camping Glair</t>
+    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) – пер. Col de Fontaines (н/к, 2696) – дер. Cheneil -- camping Glair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пер. Col de Nannaz (1А, 2773) – вер. Becca Trecare (н/к, 3032) –  пер. Col de Fontaines (н/к, 2696) – дер. Cheneil -- camping Glair</t>
   </si>
   <si>
     <t xml:space="preserve">+350,-1600</t>
@@ -256,7 +265,10 @@
     <t xml:space="preserve">13b</t>
   </si>
   <si>
-    <t xml:space="preserve">camping Glair -- St. Vincent (Casino)</t>
+    <t xml:space="preserve">кемп. Glair – дер. Buisson – дер. Grand-Moulin –  гор. St. Vincent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кемп. Glair – дер. Buisson – дер. Grand-Moulin –  переезд в гор. St. Vincent (**)</t>
   </si>
   <si>
     <t xml:space="preserve">02:00</t>
@@ -405,17 +417,17 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="32.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="32.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,7 +462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
@@ -502,7 +514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
@@ -566,7 +578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
@@ -577,7 +589,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>5.9</v>
@@ -592,24 +604,24 @@
         <v>-650</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>5.9</v>
@@ -624,24 +636,24 @@
         <v>1760</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>6.8</v>
@@ -653,27 +665,27 @@
         <v>3921.53</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>21.5</v>
@@ -685,13 +697,13 @@
         <v>3037.44</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,13 +711,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1608</v>
@@ -717,21 +729,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>17.7</v>
+        <v>10.7</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>3812</v>
@@ -743,27 +755,27 @@
         <v>2400</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>8.1</v>
+        <v>11.5</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2747</v>
@@ -772,27 +784,27 @@
         <v>3824.75</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>9.7</v>
@@ -801,37 +813,37 @@
         <v>2732.39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -841,19 +853,19 @@
     </row>
     <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>11</v>
+        <v>11.9</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>2586</v>
@@ -862,30 +874,30 @@
         <v>2768.04</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>16.9</v>
+        <v>9.3</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>1350</v>
@@ -894,10 +906,10 @@
         <v>-900</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,10 +917,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,10 +928,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>